<commit_message>
update symbolic execution evaluation
</commit_message>
<xml_diff>
--- a/symbolic-execution-engine/symbolic-execution-experiment/results/M1_vulnerable_system_calls.xlsx
+++ b/symbolic-execution-engine/symbolic-execution-experiment/results/M1_vulnerable_system_calls.xlsx
@@ -624,25 +624,25 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>semaphore_ceiling_put</t>
+          <t>timer_activate</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SEMAPHORE</t>
+          <t>TIMER</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>8,12,16</t>
+          <t>32</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>6/6</t>
         </is>
       </c>
       <c r="F8" t="inlineStr"/>
@@ -650,17 +650,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>block_allocate</t>
+          <t>semaphore_ceiling_put</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BLOCK</t>
+          <t>SEMAPHORE</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>8,16,36</t>
+          <t>8,12,16</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -668,7 +668,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>3/3</t>
         </is>
       </c>
       <c r="F9" t="inlineStr"/>
@@ -676,21 +676,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>timer_change</t>
+          <t>block_allocate</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>TIMER</t>
+          <t>BLOCK</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>8,12</t>
+          <t>8,16,36</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -702,25 +702,25 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>mutex_put</t>
+          <t>timer_change</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MUTEX</t>
+          <t>TIMER</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>8,20,24,28,40</t>
+          <t>8,12</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>8/3</t>
+          <t>2/2</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -728,25 +728,25 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>event_flags_set_notify</t>
+          <t>mutex_put</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>EVENT</t>
+          <t>MUTEX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>40,44</t>
+          <t>8,20,24,28,40</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1/1</t>
+          <t>8/3</t>
         </is>
       </c>
       <c r="F12" t="inlineStr"/>
@@ -754,25 +754,25 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>thread_priority_change</t>
+          <t>event_flags_set_notify</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>THREAD</t>
+          <t>EVENT</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>32,36,44,60,204,208</t>
+          <t>40,44</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>7/3</t>
+          <t>1/1</t>
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
@@ -780,25 +780,25 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>semaphore_put</t>
+          <t>thread_priority_change</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SEMAPHORE</t>
+          <t>THREAD</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>12,16</t>
+          <t>32,36,44,60,204,208</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>3/3</t>
+          <t>7/3</t>
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
@@ -806,25 +806,25 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>queue_flush</t>
+          <t>semaphore_put</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>QUEUE</t>
+          <t>SEMAPHORE</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>20,32,36</t>
+          <t>12,16</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>3/3</t>
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
@@ -832,17 +832,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>event_flags_create</t>
+          <t>timer_deactivate</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>EVENT</t>
+          <t>TIMER</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -850,7 +850,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1/1</t>
+          <t>6/4</t>
         </is>
       </c>
       <c r="F16" t="inlineStr"/>
@@ -858,25 +858,25 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>mutex_delete</t>
+          <t>queue_flush</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MUTEX</t>
+          <t>QUEUE</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>24,40</t>
+          <t>20,32,36</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>4/3</t>
+          <t>2/2</t>
         </is>
       </c>
       <c r="F17" t="inlineStr"/>
@@ -884,7 +884,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>event_flags_set</t>
+          <t>event_flags_create</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -894,15 +894,15 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>8,20,32</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>27/1</t>
+          <t>1/1</t>
         </is>
       </c>
       <c r="F18" t="inlineStr"/>
@@ -910,25 +910,25 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>thread_create</t>
+          <t>mutex_delete</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>THREAD</t>
+          <t>MUTEX</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>16,20,24,28,40,44,60,68,72,152,156,184,188,204,208</t>
+          <t>20,24,40</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1/1</t>
+          <t>4/3</t>
         </is>
       </c>
       <c r="F19" t="inlineStr"/>
@@ -936,25 +936,25 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>block_pool_create</t>
+          <t>event_flags_set</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BLOCK</t>
+          <t>EVENT</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>4,20,24,28</t>
+          <t>8,20,32</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1/1</t>
+          <t>27/1</t>
         </is>
       </c>
       <c r="F20" t="inlineStr"/>
@@ -962,25 +962,25 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>event_flags_get</t>
+          <t>thread_create</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>EVENT</t>
+          <t>THREAD</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>8,20,32</t>
+          <t>16,20,24,28,40,44,60,68,72,152,156,184,188,204,208</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6/4</t>
+          <t>1/1</t>
         </is>
       </c>
       <c r="F21" t="inlineStr"/>
@@ -988,21 +988,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>semaphore_create</t>
+          <t>block_pool_create</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SEMAPHORE</t>
+          <t>BLOCK</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,20,24,28</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1014,25 +1014,25 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>thread_reset</t>
+          <t>event_flags_get</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>THREAD</t>
+          <t>EVENT</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>8,20,32</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2/2</t>
+          <t>6/4</t>
         </is>
       </c>
       <c r="F23" t="inlineStr"/>
@@ -1040,7 +1040,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>semaphore_put_notify</t>
+          <t>semaphore_create</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1050,7 +1050,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>32,36</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1066,25 +1066,25 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>byte_pool_create</t>
+          <t>thread_reset</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BYTE</t>
+          <t>THREAD</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>4,8,16,20,24,28</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1/1</t>
+          <t>2/2</t>
         </is>
       </c>
       <c r="F25" t="inlineStr"/>
@@ -1092,17 +1092,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>queue_send_notify</t>
+          <t>semaphore_put_notify</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>QUEUE</t>
+          <t>SEMAPHORE</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>60,64</t>
+          <t>32,36</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1118,25 +1118,25 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>queue_front_send</t>
+          <t>timer_create</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>QUEUE</t>
+          <t>TIMER</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>16,20,32,40,44</t>
+          <t>4,8,12,20,32,44,48</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>4/3</t>
+          <t>2/1</t>
         </is>
       </c>
       <c r="F27" t="inlineStr"/>
@@ -1144,17 +1144,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>queue_receive</t>
+          <t>byte_pool_create</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>QUEUE</t>
+          <t>BYTE</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16,20,32,36,40,44</t>
+          <t>4,8,16,20,24,28</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>7/3</t>
+          <t>1/1</t>
         </is>
       </c>
       <c r="F28" t="inlineStr"/>
@@ -1170,17 +1170,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>thread_preemption_change</t>
+          <t>queue_send_notify</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>THREAD</t>
+          <t>QUEUE</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>60,208</t>
+          <t>60,64</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>5/3</t>
+          <t>1/1</t>
         </is>
       </c>
       <c r="F29" t="inlineStr"/>
@@ -1196,25 +1196,25 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>timer_activate</t>
+          <t>queue_front_send</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>TIMER</t>
+          <t>QUEUE</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>32,40,44</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>6/6</t>
+          <t>4/3</t>
         </is>
       </c>
       <c r="F30" t="inlineStr"/>
@@ -1222,25 +1222,25 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>timer_deactivate</t>
+          <t>queue_receive</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>TIMER</t>
+          <t>QUEUE</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>16,32,36,40,44</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>6/4</t>
+          <t>7/3</t>
         </is>
       </c>
       <c r="F31" t="inlineStr"/>
@@ -1248,25 +1248,25 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>timer_create</t>
+          <t>thread_preemption_change</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>TIMER</t>
+          <t>THREAD</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>4,8,12,20,32,44,48</t>
+          <t>60,208</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2/1</t>
+          <t>5/3</t>
         </is>
       </c>
       <c r="F32" t="inlineStr"/>

</xml_diff>